<commit_message>
working with implementing charts to page 1.
</commit_message>
<xml_diff>
--- a/data/kpi_df.xlsx
+++ b/data/kpi_df.xlsx
@@ -535,12 +535,12 @@
     <t>Ekonomi, administration och försäljning</t>
   </si>
   <si>
+    <t>Kultur, media och design</t>
+  </si>
+  <si>
     <t>Lantbruk, djurvård, trädgård, skog och fiske</t>
   </si>
   <si>
-    <t>Kultur, media och design</t>
-  </si>
-  <si>
     <t>Teknik och tillverkning</t>
   </si>
   <si>
@@ -550,13 +550,13 @@
     <t>Hälso- och sjukvård samt socialt arbete</t>
   </si>
   <si>
+    <t>Juridik</t>
+  </si>
+  <si>
     <t>Hotell, restaurang och turism</t>
   </si>
   <si>
     <t>Data/IT</t>
-  </si>
-  <si>
-    <t>Juridik</t>
   </si>
   <si>
     <t>Pedagogik och undervisning</t>
@@ -989,7 +989,7 @@
         <v>173</v>
       </c>
       <c r="D3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -1012,7 +1012,7 @@
         <v>174</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -1055,7 +1055,7 @@
         <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -1078,10 +1078,10 @@
         <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -1101,10 +1101,10 @@
         <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E8">
         <v>0</v>
@@ -1193,19 +1193,19 @@
         <v>12</v>
       </c>
       <c r="C12" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="D12">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E12">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F12">
-        <v>70</v>
+        <v>270</v>
       </c>
       <c r="G12">
-        <v>100</v>
+        <v>66.67</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -1216,19 +1216,19 @@
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="D13">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E13">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="F13">
-        <v>0</v>
+        <v>260</v>
       </c>
       <c r="G13">
-        <v>0</v>
+        <v>85.70999999999999</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -1239,19 +1239,19 @@
         <v>12</v>
       </c>
       <c r="C14" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="D14">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="E14">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="F14">
-        <v>270</v>
+        <v>0</v>
       </c>
       <c r="G14">
-        <v>66.67</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -1262,19 +1262,19 @@
         <v>12</v>
       </c>
       <c r="C15" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D15">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E15">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F15">
-        <v>260</v>
+        <v>140</v>
       </c>
       <c r="G15">
-        <v>85.70999999999999</v>
+        <v>66.67</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -1285,19 +1285,19 @@
         <v>12</v>
       </c>
       <c r="C16" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D16">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E16">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F16">
-        <v>230</v>
+        <v>70</v>
       </c>
       <c r="G16">
-        <v>100</v>
+        <v>66.67</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -1308,19 +1308,19 @@
         <v>12</v>
       </c>
       <c r="C17" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="D17">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="E17">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="F17">
-        <v>490</v>
+        <v>70</v>
       </c>
       <c r="G17">
-        <v>83.33</v>
+        <v>100</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -1331,19 +1331,19 @@
         <v>12</v>
       </c>
       <c r="C18" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="D18">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E18">
         <v>4</v>
       </c>
       <c r="F18">
-        <v>140</v>
+        <v>230</v>
       </c>
       <c r="G18">
-        <v>66.67</v>
+        <v>100</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -1354,19 +1354,19 @@
         <v>12</v>
       </c>
       <c r="C19" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="D19">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="E19">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="F19">
-        <v>70</v>
+        <v>490</v>
       </c>
       <c r="G19">
-        <v>66.67</v>
+        <v>83.33</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -1423,19 +1423,19 @@
         <v>13</v>
       </c>
       <c r="C22" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="D22">
         <v>1</v>
       </c>
       <c r="E22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F22">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="G22">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -1446,10 +1446,10 @@
         <v>13</v>
       </c>
       <c r="C23" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="D23">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E23">
         <v>0</v>
@@ -1469,19 +1469,19 @@
         <v>13</v>
       </c>
       <c r="C24" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F24">
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="G24">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -1607,7 +1607,7 @@
         <v>16</v>
       </c>
       <c r="C30" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D30">
         <v>4</v>
@@ -1837,10 +1837,10 @@
         <v>22</v>
       </c>
       <c r="C40" t="s">
-        <v>172</v>
+        <v>179</v>
       </c>
       <c r="D40">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E40">
         <v>0</v>
@@ -1860,10 +1860,10 @@
         <v>22</v>
       </c>
       <c r="C41" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="D41">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E41">
         <v>0</v>
@@ -1906,7 +1906,7 @@
         <v>24</v>
       </c>
       <c r="C43" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D43">
         <v>2</v>
@@ -1998,7 +1998,7 @@
         <v>26</v>
       </c>
       <c r="C47" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D47">
         <v>6</v>
@@ -2021,7 +2021,7 @@
         <v>27</v>
       </c>
       <c r="C48" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D48">
         <v>1</v>
@@ -2044,19 +2044,19 @@
         <v>27</v>
       </c>
       <c r="C49" t="s">
-        <v>172</v>
+        <v>180</v>
       </c>
       <c r="D49">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E49">
         <v>3</v>
       </c>
       <c r="F49">
-        <v>150</v>
+        <v>120</v>
       </c>
       <c r="G49">
-        <v>50</v>
+        <v>60</v>
       </c>
     </row>
     <row r="50" spans="1:7">
@@ -2067,7 +2067,7 @@
         <v>27</v>
       </c>
       <c r="C50" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="D50">
         <v>6</v>
@@ -2076,7 +2076,7 @@
         <v>3</v>
       </c>
       <c r="F50">
-        <v>220</v>
+        <v>150</v>
       </c>
       <c r="G50">
         <v>50</v>
@@ -2090,19 +2090,19 @@
         <v>27</v>
       </c>
       <c r="C51" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D51">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E51">
         <v>3</v>
       </c>
       <c r="F51">
-        <v>120</v>
+        <v>220</v>
       </c>
       <c r="G51">
-        <v>60</v>
+        <v>50</v>
       </c>
     </row>
     <row r="52" spans="1:7">
@@ -2113,19 +2113,19 @@
         <v>28</v>
       </c>
       <c r="C52" t="s">
-        <v>172</v>
+        <v>179</v>
       </c>
       <c r="D52">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E52">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F52">
-        <v>0</v>
+        <v>211</v>
       </c>
       <c r="G52">
-        <v>0</v>
+        <v>83.33</v>
       </c>
     </row>
     <row r="53" spans="1:7">
@@ -2136,19 +2136,19 @@
         <v>28</v>
       </c>
       <c r="C53" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="D53">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E53">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F53">
-        <v>211</v>
+        <v>0</v>
       </c>
       <c r="G53">
-        <v>83.33</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:7">
@@ -2182,19 +2182,19 @@
         <v>30</v>
       </c>
       <c r="C55" t="s">
-        <v>172</v>
+        <v>184</v>
       </c>
       <c r="D55">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="E55">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F55">
-        <v>160</v>
+        <v>0</v>
       </c>
       <c r="G55">
-        <v>25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:7">
@@ -2205,7 +2205,7 @@
         <v>30</v>
       </c>
       <c r="C56" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D56">
         <v>1</v>
@@ -2228,19 +2228,19 @@
         <v>30</v>
       </c>
       <c r="C57" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
       <c r="D57">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="E57">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F57">
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="G57">
-        <v>0</v>
+        <v>25</v>
       </c>
     </row>
     <row r="58" spans="1:7">
@@ -2251,7 +2251,7 @@
         <v>31</v>
       </c>
       <c r="C58" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D58">
         <v>2</v>
@@ -2274,7 +2274,7 @@
         <v>32</v>
       </c>
       <c r="C59" t="s">
-        <v>174</v>
+        <v>184</v>
       </c>
       <c r="D59">
         <v>1</v>
@@ -2297,7 +2297,7 @@
         <v>32</v>
       </c>
       <c r="C60" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="D60">
         <v>1</v>
@@ -2343,7 +2343,7 @@
         <v>32</v>
       </c>
       <c r="C62" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D62">
         <v>5</v>
@@ -2366,7 +2366,7 @@
         <v>33</v>
       </c>
       <c r="C63" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D63">
         <v>1</v>
@@ -2412,7 +2412,7 @@
         <v>35</v>
       </c>
       <c r="C65" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D65">
         <v>1</v>
@@ -2458,19 +2458,19 @@
         <v>37</v>
       </c>
       <c r="C67" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="D67">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E67">
         <v>1</v>
       </c>
       <c r="F67">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="G67">
-        <v>100</v>
+        <v>50</v>
       </c>
     </row>
     <row r="68" spans="1:7">
@@ -2481,7 +2481,7 @@
         <v>37</v>
       </c>
       <c r="C68" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="D68">
         <v>1</v>
@@ -2490,7 +2490,7 @@
         <v>1</v>
       </c>
       <c r="F68">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="G68">
         <v>100</v>
@@ -2504,19 +2504,19 @@
         <v>37</v>
       </c>
       <c r="C69" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="D69">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E69">
         <v>1</v>
       </c>
       <c r="F69">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="G69">
-        <v>50</v>
+        <v>100</v>
       </c>
     </row>
     <row r="70" spans="1:7">
@@ -2527,7 +2527,7 @@
         <v>38</v>
       </c>
       <c r="C70" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D70">
         <v>1</v>
@@ -2550,19 +2550,19 @@
         <v>39</v>
       </c>
       <c r="C71" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="D71">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E71">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F71">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="G71">
-        <v>50</v>
+        <v>0</v>
       </c>
     </row>
     <row r="72" spans="1:7">
@@ -2573,19 +2573,19 @@
         <v>39</v>
       </c>
       <c r="C72" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="D72">
         <v>1</v>
       </c>
       <c r="E72">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F72">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="G72">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="73" spans="1:7">
@@ -2596,10 +2596,10 @@
         <v>39</v>
       </c>
       <c r="C73" t="s">
-        <v>172</v>
+        <v>182</v>
       </c>
       <c r="D73">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="E73">
         <v>1</v>
@@ -2608,7 +2608,7 @@
         <v>60</v>
       </c>
       <c r="G73">
-        <v>14.29</v>
+        <v>50</v>
       </c>
     </row>
     <row r="74" spans="1:7">
@@ -2619,19 +2619,19 @@
         <v>39</v>
       </c>
       <c r="C74" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="D74">
         <v>1</v>
       </c>
       <c r="E74">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F74">
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="G74">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:7">
@@ -2642,19 +2642,19 @@
         <v>39</v>
       </c>
       <c r="C75" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="D75">
         <v>1</v>
       </c>
       <c r="E75">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F75">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="G75">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="76" spans="1:7">
@@ -2665,16 +2665,16 @@
         <v>39</v>
       </c>
       <c r="C76" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="D76">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E76">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F76">
-        <v>35</v>
+        <v>65</v>
       </c>
       <c r="G76">
         <v>100</v>
@@ -2688,19 +2688,19 @@
         <v>39</v>
       </c>
       <c r="C77" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="D77">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E77">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F77">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="G77">
-        <v>100</v>
+        <v>14.29</v>
       </c>
     </row>
     <row r="78" spans="1:7">
@@ -2711,7 +2711,7 @@
         <v>39</v>
       </c>
       <c r="C78" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="D78">
         <v>1</v>
@@ -2849,7 +2849,7 @@
         <v>43</v>
       </c>
       <c r="C84" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D84">
         <v>1</v>
@@ -2895,7 +2895,7 @@
         <v>44</v>
       </c>
       <c r="C86" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D86">
         <v>1</v>
@@ -2904,7 +2904,7 @@
         <v>1</v>
       </c>
       <c r="F86">
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="G86">
         <v>100</v>
@@ -2927,7 +2927,7 @@
         <v>1</v>
       </c>
       <c r="F87">
-        <v>120</v>
+        <v>60</v>
       </c>
       <c r="G87">
         <v>100</v>
@@ -2941,7 +2941,7 @@
         <v>45</v>
       </c>
       <c r="C88" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D88">
         <v>5</v>
@@ -3010,16 +3010,16 @@
         <v>46</v>
       </c>
       <c r="C91" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="D91">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E91">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F91">
-        <v>25</v>
+        <v>90</v>
       </c>
       <c r="G91">
         <v>100</v>
@@ -3033,19 +3033,19 @@
         <v>46</v>
       </c>
       <c r="C92" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="D92">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E92">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F92">
-        <v>60</v>
+        <v>25</v>
       </c>
       <c r="G92">
-        <v>66.67</v>
+        <v>100</v>
       </c>
     </row>
     <row r="93" spans="1:7">
@@ -3056,19 +3056,19 @@
         <v>46</v>
       </c>
       <c r="C93" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D93">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E93">
         <v>2</v>
       </c>
       <c r="F93">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="G93">
-        <v>100</v>
+        <v>66.67</v>
       </c>
     </row>
     <row r="94" spans="1:7">
@@ -3079,7 +3079,7 @@
         <v>47</v>
       </c>
       <c r="C94" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D94">
         <v>1</v>
@@ -3102,7 +3102,7 @@
         <v>48</v>
       </c>
       <c r="C95" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D95">
         <v>3</v>
@@ -3125,7 +3125,7 @@
         <v>49</v>
       </c>
       <c r="C96" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="D96">
         <v>1</v>
@@ -3148,7 +3148,7 @@
         <v>49</v>
       </c>
       <c r="C97" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="D97">
         <v>1</v>
@@ -3194,7 +3194,7 @@
         <v>50</v>
       </c>
       <c r="C99" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D99">
         <v>1</v>
@@ -3217,7 +3217,7 @@
         <v>51</v>
       </c>
       <c r="C100" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D100">
         <v>1</v>
@@ -3355,7 +3355,7 @@
         <v>56</v>
       </c>
       <c r="C106" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D106">
         <v>1</v>
@@ -3401,19 +3401,19 @@
         <v>57</v>
       </c>
       <c r="C108" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="D108">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E108">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F108">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="G108">
-        <v>0</v>
+        <v>66.67</v>
       </c>
     </row>
     <row r="109" spans="1:7">
@@ -3424,19 +3424,19 @@
         <v>57</v>
       </c>
       <c r="C109" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="D109">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E109">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F109">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="G109">
-        <v>66.67</v>
+        <v>0</v>
       </c>
     </row>
     <row r="110" spans="1:7">
@@ -3516,7 +3516,7 @@
         <v>61</v>
       </c>
       <c r="C113" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D113">
         <v>1</v>
@@ -3539,7 +3539,7 @@
         <v>61</v>
       </c>
       <c r="C114" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D114">
         <v>1</v>
@@ -3608,19 +3608,19 @@
         <v>63</v>
       </c>
       <c r="C117" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
       <c r="D117">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E117">
         <v>1</v>
       </c>
       <c r="F117">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="G117">
-        <v>20</v>
+        <v>100</v>
       </c>
     </row>
     <row r="118" spans="1:7">
@@ -3654,19 +3654,19 @@
         <v>63</v>
       </c>
       <c r="C119" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="D119">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E119">
         <v>1</v>
       </c>
       <c r="F119">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="G119">
-        <v>100</v>
+        <v>20</v>
       </c>
     </row>
     <row r="120" spans="1:7">
@@ -3677,19 +3677,19 @@
         <v>64</v>
       </c>
       <c r="C120" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="D120">
         <v>1</v>
       </c>
       <c r="E120">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F120">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="G120">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="121" spans="1:7">
@@ -3700,19 +3700,19 @@
         <v>64</v>
       </c>
       <c r="C121" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="D121">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E121">
         <v>1</v>
       </c>
       <c r="F121">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="G121">
-        <v>100</v>
+        <v>50</v>
       </c>
     </row>
     <row r="122" spans="1:7">
@@ -3723,19 +3723,19 @@
         <v>64</v>
       </c>
       <c r="C122" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D122">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E122">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F122">
-        <v>270</v>
+        <v>0</v>
       </c>
       <c r="G122">
-        <v>80</v>
+        <v>0</v>
       </c>
     </row>
     <row r="123" spans="1:7">
@@ -3746,19 +3746,19 @@
         <v>64</v>
       </c>
       <c r="C123" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D123">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E123">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F123">
-        <v>60</v>
+        <v>270</v>
       </c>
       <c r="G123">
-        <v>50</v>
+        <v>80</v>
       </c>
     </row>
     <row r="124" spans="1:7">
@@ -3792,16 +3792,16 @@
         <v>66</v>
       </c>
       <c r="C125" t="s">
-        <v>176</v>
+        <v>184</v>
       </c>
       <c r="D125">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="E125">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="F125">
-        <v>473</v>
+        <v>40</v>
       </c>
       <c r="G125">
         <v>100</v>
@@ -3815,16 +3815,16 @@
         <v>66</v>
       </c>
       <c r="C126" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="D126">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="E126">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="F126">
-        <v>60</v>
+        <v>473</v>
       </c>
       <c r="G126">
         <v>100</v>
@@ -3838,16 +3838,16 @@
         <v>66</v>
       </c>
       <c r="C127" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="D127">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E127">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="F127">
-        <v>354</v>
+        <v>60</v>
       </c>
       <c r="G127">
         <v>100</v>
@@ -3861,7 +3861,7 @@
         <v>66</v>
       </c>
       <c r="C128" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="D128">
         <v>1</v>
@@ -3870,7 +3870,7 @@
         <v>1</v>
       </c>
       <c r="F128">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="G128">
         <v>100</v>
@@ -3884,16 +3884,16 @@
         <v>66</v>
       </c>
       <c r="C129" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="D129">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E129">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F129">
-        <v>80</v>
+        <v>354</v>
       </c>
       <c r="G129">
         <v>100</v>
@@ -3930,7 +3930,7 @@
         <v>68</v>
       </c>
       <c r="C131" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D131">
         <v>7</v>
@@ -3953,19 +3953,19 @@
         <v>69</v>
       </c>
       <c r="C132" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
       <c r="D132">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E132">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F132">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="G132">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="133" spans="1:7">
@@ -3976,19 +3976,19 @@
         <v>69</v>
       </c>
       <c r="C133" t="s">
-        <v>176</v>
+        <v>185</v>
       </c>
       <c r="D133">
         <v>1</v>
       </c>
       <c r="E133">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F133">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="G133">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="134" spans="1:7">
@@ -3999,10 +3999,10 @@
         <v>69</v>
       </c>
       <c r="C134" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D134">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E134">
         <v>0</v>
@@ -4022,19 +4022,19 @@
         <v>70</v>
       </c>
       <c r="C135" t="s">
-        <v>172</v>
+        <v>181</v>
       </c>
       <c r="D135">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E135">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F135">
-        <v>140</v>
+        <v>0</v>
       </c>
       <c r="G135">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="136" spans="1:7">
@@ -4045,7 +4045,7 @@
         <v>70</v>
       </c>
       <c r="C136" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="D136">
         <v>1</v>
@@ -4068,19 +4068,19 @@
         <v>70</v>
       </c>
       <c r="C137" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="D137">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E137">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F137">
-        <v>0</v>
+        <v>140</v>
       </c>
       <c r="G137">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="138" spans="1:7">
@@ -4091,16 +4091,16 @@
         <v>71</v>
       </c>
       <c r="C138" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="D138">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E138">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F138">
-        <v>140</v>
+        <v>515</v>
       </c>
       <c r="G138">
         <v>100</v>
@@ -4137,19 +4137,19 @@
         <v>71</v>
       </c>
       <c r="C140" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="D140">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="E140">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="F140">
-        <v>100</v>
+        <v>424</v>
       </c>
       <c r="G140">
-        <v>75</v>
+        <v>80</v>
       </c>
     </row>
     <row r="141" spans="1:7">
@@ -4160,16 +4160,16 @@
         <v>71</v>
       </c>
       <c r="C141" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
       <c r="D141">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E141">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F141">
-        <v>515</v>
+        <v>140</v>
       </c>
       <c r="G141">
         <v>100</v>
@@ -4183,19 +4183,19 @@
         <v>71</v>
       </c>
       <c r="C142" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="D142">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="E142">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="F142">
-        <v>424</v>
+        <v>100</v>
       </c>
       <c r="G142">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="143" spans="1:7">
@@ -4206,19 +4206,19 @@
         <v>72</v>
       </c>
       <c r="C143" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="D143">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E143">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F143">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="G143">
-        <v>0</v>
+        <v>50</v>
       </c>
     </row>
     <row r="144" spans="1:7">
@@ -4229,19 +4229,19 @@
         <v>72</v>
       </c>
       <c r="C144" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
       <c r="D144">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E144">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F144">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="G144">
-        <v>50</v>
+        <v>0</v>
       </c>
     </row>
     <row r="145" spans="1:7">
@@ -4252,19 +4252,19 @@
         <v>73</v>
       </c>
       <c r="C145" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="D145">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E145">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F145">
-        <v>220</v>
+        <v>0</v>
       </c>
       <c r="G145">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="146" spans="1:7">
@@ -4275,19 +4275,19 @@
         <v>73</v>
       </c>
       <c r="C146" t="s">
-        <v>172</v>
+        <v>181</v>
       </c>
       <c r="D146">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E146">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F146">
-        <v>0</v>
+        <v>95</v>
       </c>
       <c r="G146">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="147" spans="1:7">
@@ -4298,16 +4298,16 @@
         <v>73</v>
       </c>
       <c r="C147" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="D147">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E147">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F147">
-        <v>95</v>
+        <v>220</v>
       </c>
       <c r="G147">
         <v>100</v>
@@ -4324,16 +4324,16 @@
         <v>174</v>
       </c>
       <c r="D148">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E148">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F148">
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="G148">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="149" spans="1:7">
@@ -4347,16 +4347,16 @@
         <v>173</v>
       </c>
       <c r="D149">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E149">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F149">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="G149">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="150" spans="1:7">
@@ -4390,19 +4390,19 @@
         <v>76</v>
       </c>
       <c r="C151" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D151">
         <v>1</v>
       </c>
       <c r="E151">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F151">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="G151">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="152" spans="1:7">
@@ -4413,7 +4413,7 @@
         <v>76</v>
       </c>
       <c r="C152" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="D152">
         <v>1</v>
@@ -4436,19 +4436,19 @@
         <v>76</v>
       </c>
       <c r="C153" t="s">
-        <v>175</v>
+        <v>184</v>
       </c>
       <c r="D153">
         <v>1</v>
       </c>
       <c r="E153">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F153">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="G153">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="154" spans="1:7">
@@ -4459,19 +4459,19 @@
         <v>77</v>
       </c>
       <c r="C154" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D154">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E154">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F154">
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="G154">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="155" spans="1:7">
@@ -4482,16 +4482,16 @@
         <v>77</v>
       </c>
       <c r="C155" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="D155">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E155">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F155">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="G155">
         <v>100</v>
@@ -4505,10 +4505,10 @@
         <v>77</v>
       </c>
       <c r="C156" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="D156">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E156">
         <v>0</v>
@@ -4528,16 +4528,16 @@
         <v>77</v>
       </c>
       <c r="C157" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
       <c r="D157">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E157">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F157">
-        <v>315</v>
+        <v>100</v>
       </c>
       <c r="G157">
         <v>100</v>
@@ -4551,19 +4551,19 @@
         <v>77</v>
       </c>
       <c r="C158" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="D158">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E158">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F158">
-        <v>0</v>
+        <v>315</v>
       </c>
       <c r="G158">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="159" spans="1:7">
@@ -4574,7 +4574,7 @@
         <v>78</v>
       </c>
       <c r="C159" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D159">
         <v>2</v>
@@ -4643,7 +4643,7 @@
         <v>80</v>
       </c>
       <c r="C162" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D162">
         <v>1</v>
@@ -4666,7 +4666,7 @@
         <v>80</v>
       </c>
       <c r="C163" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D163">
         <v>1</v>
@@ -4758,19 +4758,19 @@
         <v>82</v>
       </c>
       <c r="C167" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D167">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E167">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F167">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="G167">
-        <v>50</v>
+        <v>66.67</v>
       </c>
     </row>
     <row r="168" spans="1:7">
@@ -4781,19 +4781,19 @@
         <v>82</v>
       </c>
       <c r="C168" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D168">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E168">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F168">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="G168">
-        <v>66.67</v>
+        <v>50</v>
       </c>
     </row>
     <row r="169" spans="1:7">
@@ -4804,19 +4804,19 @@
         <v>83</v>
       </c>
       <c r="C169" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
       <c r="D169">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E169">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F169">
-        <v>0</v>
+        <v>210</v>
       </c>
       <c r="G169">
-        <v>0</v>
+        <v>42.86</v>
       </c>
     </row>
     <row r="170" spans="1:7">
@@ -4827,7 +4827,7 @@
         <v>83</v>
       </c>
       <c r="C170" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D170">
         <v>1</v>
@@ -4873,19 +4873,19 @@
         <v>83</v>
       </c>
       <c r="C172" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="D172">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E172">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F172">
-        <v>210</v>
+        <v>0</v>
       </c>
       <c r="G172">
-        <v>42.86</v>
+        <v>0</v>
       </c>
     </row>
     <row r="173" spans="1:7">
@@ -4919,19 +4919,19 @@
         <v>85</v>
       </c>
       <c r="C174" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="D174">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E174">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="F174">
-        <v>540</v>
+        <v>75</v>
       </c>
       <c r="G174">
-        <v>100</v>
+        <v>66.67</v>
       </c>
     </row>
     <row r="175" spans="1:7">
@@ -4942,19 +4942,19 @@
         <v>85</v>
       </c>
       <c r="C175" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="D175">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E175">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="F175">
-        <v>75</v>
+        <v>540</v>
       </c>
       <c r="G175">
-        <v>66.67</v>
+        <v>100</v>
       </c>
     </row>
     <row r="176" spans="1:7">
@@ -5034,19 +5034,19 @@
         <v>89</v>
       </c>
       <c r="C179" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
       <c r="D179">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E179">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F179">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="G179">
-        <v>50</v>
+        <v>0</v>
       </c>
     </row>
     <row r="180" spans="1:7">
@@ -5080,19 +5080,19 @@
         <v>89</v>
       </c>
       <c r="C181" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="D181">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E181">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F181">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="G181">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="182" spans="1:7">
@@ -5103,19 +5103,19 @@
         <v>89</v>
       </c>
       <c r="C182" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="D182">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E182">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F182">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="G182">
-        <v>100</v>
+        <v>33.33</v>
       </c>
     </row>
     <row r="183" spans="1:7">
@@ -5126,19 +5126,19 @@
         <v>89</v>
       </c>
       <c r="C183" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="D183">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E183">
         <v>1</v>
       </c>
       <c r="F183">
-        <v>70</v>
+        <v>35</v>
       </c>
       <c r="G183">
-        <v>33.33</v>
+        <v>50</v>
       </c>
     </row>
     <row r="184" spans="1:7">
@@ -5218,7 +5218,7 @@
         <v>91</v>
       </c>
       <c r="C187" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
       <c r="D187">
         <v>1</v>
@@ -5241,10 +5241,10 @@
         <v>91</v>
       </c>
       <c r="C188" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="D188">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E188">
         <v>0</v>
@@ -5264,10 +5264,10 @@
         <v>91</v>
       </c>
       <c r="C189" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="D189">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E189">
         <v>0</v>
@@ -5287,19 +5287,19 @@
         <v>92</v>
       </c>
       <c r="C190" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="D190">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E190">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F190">
-        <v>0</v>
+        <v>140</v>
       </c>
       <c r="G190">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="191" spans="1:7">
@@ -5310,19 +5310,19 @@
         <v>92</v>
       </c>
       <c r="C191" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="D191">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E191">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F191">
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="G191">
-        <v>50</v>
+        <v>0</v>
       </c>
     </row>
     <row r="192" spans="1:7">
@@ -5333,19 +5333,19 @@
         <v>92</v>
       </c>
       <c r="C192" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="D192">
         <v>2</v>
       </c>
       <c r="E192">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F192">
-        <v>140</v>
+        <v>70</v>
       </c>
       <c r="G192">
-        <v>100</v>
+        <v>50</v>
       </c>
     </row>
     <row r="193" spans="1:7">
@@ -5356,19 +5356,19 @@
         <v>93</v>
       </c>
       <c r="C193" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="D193">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E193">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F193">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="G193">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="194" spans="1:7">
@@ -5379,19 +5379,19 @@
         <v>93</v>
       </c>
       <c r="C194" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
       <c r="D194">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E194">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F194">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="G194">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="195" spans="1:7">
@@ -5425,19 +5425,19 @@
         <v>95</v>
       </c>
       <c r="C196" t="s">
-        <v>173</v>
+        <v>181</v>
       </c>
       <c r="D196">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E196">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F196">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="G196">
-        <v>50</v>
+        <v>0</v>
       </c>
     </row>
     <row r="197" spans="1:7">
@@ -5471,19 +5471,19 @@
         <v>95</v>
       </c>
       <c r="C198" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="D198">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E198">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F198">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="G198">
-        <v>0</v>
+        <v>50</v>
       </c>
     </row>
     <row r="199" spans="1:7">
@@ -5540,19 +5540,19 @@
         <v>97</v>
       </c>
       <c r="C201" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D201">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E201">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F201">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="G201">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="202" spans="1:7">
@@ -5563,19 +5563,19 @@
         <v>97</v>
       </c>
       <c r="C202" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="D202">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E202">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F202">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="G202">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="203" spans="1:7">
@@ -5632,7 +5632,7 @@
         <v>99</v>
       </c>
       <c r="C205" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D205">
         <v>7</v>
@@ -5655,7 +5655,7 @@
         <v>100</v>
       </c>
       <c r="C206" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D206">
         <v>5</v>
@@ -5678,7 +5678,7 @@
         <v>100</v>
       </c>
       <c r="C207" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D207">
         <v>1</v>
@@ -5724,19 +5724,19 @@
         <v>101</v>
       </c>
       <c r="C209" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D209">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E209">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F209">
-        <v>120</v>
+        <v>50</v>
       </c>
       <c r="G209">
-        <v>60</v>
+        <v>50</v>
       </c>
     </row>
     <row r="210" spans="1:7">
@@ -5747,19 +5747,19 @@
         <v>101</v>
       </c>
       <c r="C210" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="D210">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E210">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F210">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="G210">
-        <v>0</v>
+        <v>60</v>
       </c>
     </row>
     <row r="211" spans="1:7">
@@ -5770,19 +5770,19 @@
         <v>101</v>
       </c>
       <c r="C211" t="s">
-        <v>175</v>
+        <v>182</v>
       </c>
       <c r="D211">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E211">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F211">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="G211">
-        <v>50</v>
+        <v>0</v>
       </c>
     </row>
     <row r="212" spans="1:7">
@@ -5793,19 +5793,19 @@
         <v>102</v>
       </c>
       <c r="C212" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="D212">
         <v>1</v>
       </c>
       <c r="E212">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F212">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="G212">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="213" spans="1:7">
@@ -5816,19 +5816,19 @@
         <v>102</v>
       </c>
       <c r="C213" t="s">
-        <v>172</v>
+        <v>180</v>
       </c>
       <c r="D213">
-        <v>26</v>
+        <v>1</v>
       </c>
       <c r="E213">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="F213">
-        <v>1920</v>
+        <v>80</v>
       </c>
       <c r="G213">
-        <v>92.31</v>
+        <v>100</v>
       </c>
     </row>
     <row r="214" spans="1:7">
@@ -5839,19 +5839,19 @@
         <v>102</v>
       </c>
       <c r="C214" t="s">
-        <v>174</v>
+        <v>184</v>
       </c>
       <c r="D214">
         <v>1</v>
       </c>
       <c r="E214">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F214">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="G214">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="215" spans="1:7">
@@ -5862,7 +5862,7 @@
         <v>102</v>
       </c>
       <c r="C215" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D215">
         <v>1</v>
@@ -5885,19 +5885,19 @@
         <v>102</v>
       </c>
       <c r="C216" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
       <c r="D216">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="E216">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="F216">
-        <v>40</v>
+        <v>1920</v>
       </c>
       <c r="G216">
-        <v>100</v>
+        <v>92.31</v>
       </c>
     </row>
     <row r="217" spans="1:7">
@@ -5977,7 +5977,7 @@
         <v>106</v>
       </c>
       <c r="C220" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D220">
         <v>2</v>
@@ -6023,7 +6023,7 @@
         <v>107</v>
       </c>
       <c r="C222" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D222">
         <v>1</v>
@@ -6046,19 +6046,19 @@
         <v>108</v>
       </c>
       <c r="C223" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D223">
         <v>1</v>
       </c>
       <c r="E223">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F223">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="G223">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="224" spans="1:7">
@@ -6069,19 +6069,19 @@
         <v>108</v>
       </c>
       <c r="C224" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D224">
         <v>1</v>
       </c>
       <c r="E224">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F224">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="G224">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="225" spans="1:7">
@@ -6115,19 +6115,19 @@
         <v>109</v>
       </c>
       <c r="C226" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D226">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E226">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F226">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="G226">
-        <v>0</v>
+        <v>50</v>
       </c>
     </row>
     <row r="227" spans="1:7">
@@ -6138,10 +6138,10 @@
         <v>109</v>
       </c>
       <c r="C227" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="D227">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E227">
         <v>1</v>
@@ -6150,7 +6150,7 @@
         <v>60</v>
       </c>
       <c r="G227">
-        <v>50</v>
+        <v>100</v>
       </c>
     </row>
     <row r="228" spans="1:7">
@@ -6161,19 +6161,19 @@
         <v>109</v>
       </c>
       <c r="C228" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="D228">
         <v>1</v>
       </c>
       <c r="E228">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F228">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="G228">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="229" spans="1:7">
@@ -6184,19 +6184,19 @@
         <v>110</v>
       </c>
       <c r="C229" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="D229">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E229">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F229">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="G229">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="230" spans="1:7">
@@ -6207,19 +6207,19 @@
         <v>110</v>
       </c>
       <c r="C230" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D230">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E230">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F230">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="G230">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="231" spans="1:7">
@@ -6230,7 +6230,7 @@
         <v>111</v>
       </c>
       <c r="C231" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D231">
         <v>1</v>
@@ -6276,7 +6276,7 @@
         <v>111</v>
       </c>
       <c r="C233" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D233">
         <v>3</v>
@@ -6322,7 +6322,7 @@
         <v>112</v>
       </c>
       <c r="C235" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D235">
         <v>1</v>
@@ -6368,19 +6368,19 @@
         <v>114</v>
       </c>
       <c r="C237" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D237">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E237">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F237">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="G237">
-        <v>0</v>
+        <v>50</v>
       </c>
     </row>
     <row r="238" spans="1:7">
@@ -6391,19 +6391,19 @@
         <v>114</v>
       </c>
       <c r="C238" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D238">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E238">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F238">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="G238">
-        <v>50</v>
+        <v>0</v>
       </c>
     </row>
     <row r="239" spans="1:7">
@@ -6414,7 +6414,7 @@
         <v>115</v>
       </c>
       <c r="C239" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="D239">
         <v>1</v>
@@ -6437,7 +6437,7 @@
         <v>115</v>
       </c>
       <c r="C240" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="D240">
         <v>1</v>
@@ -6460,7 +6460,7 @@
         <v>116</v>
       </c>
       <c r="C241" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D241">
         <v>1</v>
@@ -6483,7 +6483,7 @@
         <v>116</v>
       </c>
       <c r="C242" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="D242">
         <v>1</v>
@@ -6506,7 +6506,7 @@
         <v>116</v>
       </c>
       <c r="C243" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D243">
         <v>1</v>
@@ -6529,7 +6529,7 @@
         <v>116</v>
       </c>
       <c r="C244" t="s">
-        <v>172</v>
+        <v>181</v>
       </c>
       <c r="D244">
         <v>1</v>
@@ -6575,7 +6575,7 @@
         <v>117</v>
       </c>
       <c r="C246" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D246">
         <v>3</v>
@@ -6621,19 +6621,19 @@
         <v>119</v>
       </c>
       <c r="C248" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="D248">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E248">
         <v>1</v>
       </c>
       <c r="F248">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="G248">
-        <v>50</v>
+        <v>100</v>
       </c>
     </row>
     <row r="249" spans="1:7">
@@ -6644,16 +6644,16 @@
         <v>119</v>
       </c>
       <c r="C249" t="s">
-        <v>175</v>
+        <v>182</v>
       </c>
       <c r="D249">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E249">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F249">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="G249">
         <v>50</v>
@@ -6667,19 +6667,19 @@
         <v>119</v>
       </c>
       <c r="C250" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="D250">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E250">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F250">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="G250">
-        <v>50</v>
+        <v>100</v>
       </c>
     </row>
     <row r="251" spans="1:7">
@@ -6690,19 +6690,19 @@
         <v>119</v>
       </c>
       <c r="C251" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="D251">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E251">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F251">
-        <v>0</v>
+        <v>65</v>
       </c>
       <c r="G251">
-        <v>0</v>
+        <v>50</v>
       </c>
     </row>
     <row r="252" spans="1:7">
@@ -6713,19 +6713,19 @@
         <v>119</v>
       </c>
       <c r="C252" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="D252">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E252">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F252">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="G252">
-        <v>50</v>
+        <v>0</v>
       </c>
     </row>
     <row r="253" spans="1:7">
@@ -6736,19 +6736,19 @@
         <v>119</v>
       </c>
       <c r="C253" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="D253">
         <v>2</v>
       </c>
       <c r="E253">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F253">
-        <v>53</v>
+        <v>27</v>
       </c>
       <c r="G253">
-        <v>100</v>
+        <v>50</v>
       </c>
     </row>
     <row r="254" spans="1:7">
@@ -6759,19 +6759,19 @@
         <v>119</v>
       </c>
       <c r="C254" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D254">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E254">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F254">
-        <v>0</v>
+        <v>72</v>
       </c>
       <c r="G254">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="255" spans="1:7">
@@ -6782,7 +6782,7 @@
         <v>119</v>
       </c>
       <c r="C255" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D255">
         <v>2</v>
@@ -6791,7 +6791,7 @@
         <v>1</v>
       </c>
       <c r="F255">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="G255">
         <v>50</v>
@@ -6805,19 +6805,19 @@
         <v>119</v>
       </c>
       <c r="C256" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D256">
         <v>1</v>
       </c>
       <c r="E256">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F256">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="G256">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="257" spans="1:7">
@@ -6828,19 +6828,19 @@
         <v>119</v>
       </c>
       <c r="C257" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="D257">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E257">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F257">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="G257">
-        <v>100</v>
+        <v>50</v>
       </c>
     </row>
     <row r="258" spans="1:7">
@@ -6851,7 +6851,7 @@
         <v>120</v>
       </c>
       <c r="C258" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D258">
         <v>2</v>
@@ -6874,19 +6874,19 @@
         <v>121</v>
       </c>
       <c r="C259" t="s">
-        <v>172</v>
+        <v>180</v>
       </c>
       <c r="D259">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E259">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F259">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="G259">
-        <v>0</v>
+        <v>50</v>
       </c>
     </row>
     <row r="260" spans="1:7">
@@ -6897,19 +6897,19 @@
         <v>121</v>
       </c>
       <c r="C260" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="D260">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E260">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F260">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="G260">
-        <v>50</v>
+        <v>0</v>
       </c>
     </row>
     <row r="261" spans="1:7">
@@ -6920,10 +6920,10 @@
         <v>122</v>
       </c>
       <c r="C261" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="D261">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E261">
         <v>0</v>
@@ -6943,10 +6943,10 @@
         <v>122</v>
       </c>
       <c r="C262" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D262">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E262">
         <v>0</v>
@@ -6966,19 +6966,19 @@
         <v>123</v>
       </c>
       <c r="C263" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="D263">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E263">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F263">
-        <v>140</v>
+        <v>210</v>
       </c>
       <c r="G263">
-        <v>50</v>
+        <v>75</v>
       </c>
     </row>
     <row r="264" spans="1:7">
@@ -6989,7 +6989,7 @@
         <v>123</v>
       </c>
       <c r="C264" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D264">
         <v>1</v>
@@ -7012,19 +7012,19 @@
         <v>123</v>
       </c>
       <c r="C265" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="D265">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E265">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F265">
-        <v>210</v>
+        <v>170</v>
       </c>
       <c r="G265">
-        <v>75</v>
+        <v>66.67</v>
       </c>
     </row>
     <row r="266" spans="1:7">
@@ -7035,19 +7035,19 @@
         <v>123</v>
       </c>
       <c r="C266" t="s">
-        <v>172</v>
+        <v>180</v>
       </c>
       <c r="D266">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E266">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F266">
-        <v>170</v>
+        <v>140</v>
       </c>
       <c r="G266">
-        <v>66.67</v>
+        <v>50</v>
       </c>
     </row>
     <row r="267" spans="1:7">
@@ -7081,19 +7081,19 @@
         <v>124</v>
       </c>
       <c r="C268" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="D268">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E268">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F268">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G268">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="269" spans="1:7">
@@ -7104,19 +7104,19 @@
         <v>124</v>
       </c>
       <c r="C269" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="D269">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E269">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F269">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G269">
-        <v>0</v>
+        <v>50</v>
       </c>
     </row>
     <row r="270" spans="1:7">
@@ -7136,7 +7136,7 @@
         <v>1</v>
       </c>
       <c r="F270">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="G270">
         <v>50</v>
@@ -7150,19 +7150,19 @@
         <v>124</v>
       </c>
       <c r="C271" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="D271">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E271">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F271">
-        <v>25</v>
+        <v>100</v>
       </c>
       <c r="G271">
-        <v>50</v>
+        <v>100</v>
       </c>
     </row>
     <row r="272" spans="1:7">
@@ -7265,7 +7265,7 @@
         <v>128</v>
       </c>
       <c r="C276" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D276">
         <v>4</v>
@@ -7288,19 +7288,19 @@
         <v>129</v>
       </c>
       <c r="C277" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="D277">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E277">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F277">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="G277">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="278" spans="1:7">
@@ -7311,19 +7311,19 @@
         <v>129</v>
       </c>
       <c r="C278" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D278">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E278">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F278">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="G278">
-        <v>75</v>
+        <v>0</v>
       </c>
     </row>
     <row r="279" spans="1:7">
@@ -7334,19 +7334,19 @@
         <v>129</v>
       </c>
       <c r="C279" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="D279">
+        <v>4</v>
+      </c>
+      <c r="E279">
         <v>3</v>
       </c>
-      <c r="E279">
-        <v>0</v>
-      </c>
       <c r="F279">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="G279">
-        <v>0</v>
+        <v>75</v>
       </c>
     </row>
     <row r="280" spans="1:7">
@@ -7357,16 +7357,16 @@
         <v>129</v>
       </c>
       <c r="C280" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="D280">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E280">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F280">
-        <v>44</v>
+        <v>20</v>
       </c>
       <c r="G280">
         <v>100</v>
@@ -7380,19 +7380,19 @@
         <v>129</v>
       </c>
       <c r="C281" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="D281">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E281">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F281">
-        <v>100</v>
+        <v>160</v>
       </c>
       <c r="G281">
-        <v>100</v>
+        <v>66.67</v>
       </c>
     </row>
     <row r="282" spans="1:7">
@@ -7403,19 +7403,19 @@
         <v>129</v>
       </c>
       <c r="C282" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="D282">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E282">
         <v>2</v>
       </c>
       <c r="F282">
-        <v>160</v>
+        <v>44</v>
       </c>
       <c r="G282">
-        <v>66.67</v>
+        <v>100</v>
       </c>
     </row>
     <row r="283" spans="1:7">
@@ -7426,19 +7426,19 @@
         <v>129</v>
       </c>
       <c r="C283" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D283">
         <v>1</v>
       </c>
       <c r="E283">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F283">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G283">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="284" spans="1:7">
@@ -7449,7 +7449,7 @@
         <v>130</v>
       </c>
       <c r="C284" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D284">
         <v>1</v>
@@ -7587,7 +7587,7 @@
         <v>135</v>
       </c>
       <c r="C290" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D290">
         <v>1</v>
@@ -7610,7 +7610,7 @@
         <v>136</v>
       </c>
       <c r="C291" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D291">
         <v>1</v>
@@ -7633,7 +7633,7 @@
         <v>137</v>
       </c>
       <c r="C292" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D292">
         <v>6</v>
@@ -7656,7 +7656,7 @@
         <v>138</v>
       </c>
       <c r="C293" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D293">
         <v>3</v>
@@ -7702,19 +7702,19 @@
         <v>140</v>
       </c>
       <c r="C295" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="D295">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E295">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F295">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G295">
-        <v>33.33</v>
+        <v>0</v>
       </c>
     </row>
     <row r="296" spans="1:7">
@@ -7725,19 +7725,19 @@
         <v>140</v>
       </c>
       <c r="C296" t="s">
-        <v>172</v>
+        <v>180</v>
       </c>
       <c r="D296">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E296">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F296">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G296">
-        <v>0</v>
+        <v>33.33</v>
       </c>
     </row>
     <row r="297" spans="1:7">
@@ -7771,19 +7771,19 @@
         <v>141</v>
       </c>
       <c r="C298" t="s">
-        <v>172</v>
+        <v>180</v>
       </c>
       <c r="D298">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E298">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F298">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="G298">
-        <v>50</v>
+        <v>0</v>
       </c>
     </row>
     <row r="299" spans="1:7">
@@ -7794,19 +7794,19 @@
         <v>141</v>
       </c>
       <c r="C299" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="D299">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E299">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F299">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="G299">
-        <v>0</v>
+        <v>50</v>
       </c>
     </row>
     <row r="300" spans="1:7">
@@ -7817,19 +7817,19 @@
         <v>142</v>
       </c>
       <c r="C300" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="D300">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E300">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F300">
-        <v>80</v>
+        <v>160</v>
       </c>
       <c r="G300">
-        <v>100</v>
+        <v>75</v>
       </c>
     </row>
     <row r="301" spans="1:7">
@@ -7840,19 +7840,19 @@
         <v>142</v>
       </c>
       <c r="C301" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="D301">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E301">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F301">
-        <v>160</v>
+        <v>80</v>
       </c>
       <c r="G301">
-        <v>75</v>
+        <v>100</v>
       </c>
     </row>
     <row r="302" spans="1:7">
@@ -7863,7 +7863,7 @@
         <v>143</v>
       </c>
       <c r="C302" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D302">
         <v>5</v>
@@ -7886,7 +7886,7 @@
         <v>144</v>
       </c>
       <c r="C303" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D303">
         <v>3</v>
@@ -7912,16 +7912,16 @@
         <v>180</v>
       </c>
       <c r="D304">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E304">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F304">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="G304">
-        <v>0</v>
+        <v>33.33</v>
       </c>
     </row>
     <row r="305" spans="1:7">
@@ -7932,19 +7932,19 @@
         <v>145</v>
       </c>
       <c r="C305" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D305">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E305">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F305">
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="G305">
-        <v>33.33</v>
+        <v>0</v>
       </c>
     </row>
     <row r="306" spans="1:7">
@@ -7955,7 +7955,7 @@
         <v>146</v>
       </c>
       <c r="C306" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D306">
         <v>3</v>
@@ -8024,7 +8024,7 @@
         <v>149</v>
       </c>
       <c r="C309" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D309">
         <v>1</v>
@@ -8096,16 +8096,16 @@
         <v>180</v>
       </c>
       <c r="D312">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E312">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F312">
-        <v>0</v>
+        <v>115</v>
       </c>
       <c r="G312">
-        <v>0</v>
+        <v>60</v>
       </c>
     </row>
     <row r="313" spans="1:7">
@@ -8116,19 +8116,19 @@
         <v>151</v>
       </c>
       <c r="C313" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D313">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E313">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F313">
-        <v>115</v>
+        <v>0</v>
       </c>
       <c r="G313">
-        <v>60</v>
+        <v>0</v>
       </c>
     </row>
     <row r="314" spans="1:7">
@@ -8139,7 +8139,7 @@
         <v>152</v>
       </c>
       <c r="C314" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="D314">
         <v>1</v>
@@ -8162,7 +8162,7 @@
         <v>152</v>
       </c>
       <c r="C315" t="s">
-        <v>172</v>
+        <v>180</v>
       </c>
       <c r="D315">
         <v>1</v>
@@ -8185,7 +8185,7 @@
         <v>152</v>
       </c>
       <c r="C316" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D316">
         <v>1</v>
@@ -8208,7 +8208,7 @@
         <v>153</v>
       </c>
       <c r="C317" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D317">
         <v>1</v>
@@ -8277,19 +8277,19 @@
         <v>155</v>
       </c>
       <c r="C320" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D320">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E320">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F320">
-        <v>155</v>
+        <v>50</v>
       </c>
       <c r="G320">
-        <v>100</v>
+        <v>50</v>
       </c>
     </row>
     <row r="321" spans="1:7">
@@ -8300,16 +8300,16 @@
         <v>155</v>
       </c>
       <c r="C321" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="D321">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E321">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F321">
-        <v>24</v>
+        <v>155</v>
       </c>
       <c r="G321">
         <v>100</v>
@@ -8323,19 +8323,19 @@
         <v>155</v>
       </c>
       <c r="C322" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="D322">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E322">
         <v>1</v>
       </c>
       <c r="F322">
-        <v>50</v>
+        <v>24</v>
       </c>
       <c r="G322">
-        <v>50</v>
+        <v>100</v>
       </c>
     </row>
     <row r="323" spans="1:7">
@@ -8415,7 +8415,7 @@
         <v>158</v>
       </c>
       <c r="C326" t="s">
-        <v>172</v>
+        <v>179</v>
       </c>
       <c r="D326">
         <v>1</v>
@@ -8424,7 +8424,7 @@
         <v>1</v>
       </c>
       <c r="F326">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="G326">
         <v>100</v>
@@ -8438,19 +8438,19 @@
         <v>158</v>
       </c>
       <c r="C327" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="D327">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E327">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F327">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="G327">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="328" spans="1:7">
@@ -8461,19 +8461,19 @@
         <v>158</v>
       </c>
       <c r="C328" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="D328">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E328">
         <v>1</v>
       </c>
       <c r="F328">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="G328">
-        <v>50</v>
+        <v>100</v>
       </c>
     </row>
     <row r="329" spans="1:7">
@@ -8484,19 +8484,19 @@
         <v>158</v>
       </c>
       <c r="C329" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="D329">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E329">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F329">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G329">
-        <v>0</v>
+        <v>50</v>
       </c>
     </row>
     <row r="330" spans="1:7">
@@ -8507,19 +8507,19 @@
         <v>159</v>
       </c>
       <c r="C330" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="D330">
         <v>3</v>
       </c>
       <c r="E330">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F330">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="G330">
-        <v>66.67</v>
+        <v>0</v>
       </c>
     </row>
     <row r="331" spans="1:7">
@@ -8530,10 +8530,10 @@
         <v>159</v>
       </c>
       <c r="C331" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
       <c r="D331">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E331">
         <v>0</v>
@@ -8553,19 +8553,19 @@
         <v>159</v>
       </c>
       <c r="C332" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D332">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E332">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F332">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="G332">
-        <v>0</v>
+        <v>66.67</v>
       </c>
     </row>
     <row r="333" spans="1:7">
@@ -8622,7 +8622,7 @@
         <v>162</v>
       </c>
       <c r="C335" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D335">
         <v>1</v>
@@ -8645,7 +8645,7 @@
         <v>162</v>
       </c>
       <c r="C336" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D336">
         <v>1</v>
@@ -8760,19 +8760,19 @@
         <v>165</v>
       </c>
       <c r="C341" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
       <c r="D341">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E341">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F341">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="G341">
-        <v>0</v>
+        <v>50</v>
       </c>
     </row>
     <row r="342" spans="1:7">
@@ -8783,19 +8783,19 @@
         <v>165</v>
       </c>
       <c r="C342" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="D342">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E342">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F342">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="G342">
-        <v>50</v>
+        <v>0</v>
       </c>
     </row>
     <row r="343" spans="1:7">
@@ -8806,7 +8806,7 @@
         <v>165</v>
       </c>
       <c r="C343" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D343">
         <v>2</v>
@@ -8829,19 +8829,19 @@
         <v>165</v>
       </c>
       <c r="C344" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D344">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E344">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F344">
-        <v>218</v>
+        <v>0</v>
       </c>
       <c r="G344">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="345" spans="1:7">
@@ -8852,19 +8852,19 @@
         <v>165</v>
       </c>
       <c r="C345" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D345">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E345">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F345">
-        <v>0</v>
+        <v>218</v>
       </c>
       <c r="G345">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="346" spans="1:7">
@@ -8875,10 +8875,10 @@
         <v>166</v>
       </c>
       <c r="C346" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="D346">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E346">
         <v>0</v>
@@ -8898,10 +8898,10 @@
         <v>166</v>
       </c>
       <c r="C347" t="s">
-        <v>172</v>
+        <v>179</v>
       </c>
       <c r="D347">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E347">
         <v>0</v>
@@ -8921,7 +8921,7 @@
         <v>167</v>
       </c>
       <c r="C348" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D348">
         <v>6</v>
@@ -8990,16 +8990,16 @@
         <v>169</v>
       </c>
       <c r="C351" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D351">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E351">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F351">
-        <v>110</v>
+        <v>80</v>
       </c>
       <c r="G351">
         <v>100</v>
@@ -9013,16 +9013,16 @@
         <v>169</v>
       </c>
       <c r="C352" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="D352">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E352">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F352">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="G352">
         <v>100</v>
@@ -9036,16 +9036,16 @@
         <v>169</v>
       </c>
       <c r="C353" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="D353">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E353">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F353">
-        <v>40</v>
+        <v>110</v>
       </c>
       <c r="G353">
         <v>100</v>
@@ -9059,7 +9059,7 @@
         <v>170</v>
       </c>
       <c r="C354" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D354">
         <v>1</v>

</xml_diff>